<commit_message>
Examples: Added Example setup table for 8k processing
</commit_message>
<xml_diff>
--- a/Example_Files/Template; Compound Setup Table 8K Up to 48 Compunds 6 Point Dose.xlsx
+++ b/Example_Files/Template; Compound Setup Table 8K Up to 48 Compunds 6 Point Dose.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bfulroth/GitProjects/SPR_Create_Dotmatics_ADLP_File/Example_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2E9CBB-A702-E74D-81DC-BDECA1372FF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6FB508-C243-474B-98EF-699AA38499EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32640" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="5080" windowWidth="32640" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Table 1-1-1-1" sheetId="1" r:id="rId1"/>
@@ -335,7 +335,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -365,6 +365,13 @@
       <color indexed="8"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -709,7 +716,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -908,6 +915,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2068,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1"/>
@@ -2085,13 +2095,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.75" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="67" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -2100,10 +2110,10 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="67" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -2121,13 +2131,13 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="67" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="2" t="s">

</xml_diff>